<commit_message>
Deleted old model files, updated docs and cleaning code
</commit_message>
<xml_diff>
--- a/creating_train_test_data/label_correction.xlsx
+++ b/creating_train_test_data/label_correction.xlsx
@@ -20,71 +20,149 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="207">
   <si>
     <t>index</t>
   </si>
   <si>
+    <t>Speleothem</t>
+  </si>
+  <si>
+    <t>LakeSediment</t>
+  </si>
+  <si>
     <t>GlacierIce</t>
   </si>
   <si>
     <t>Wood</t>
   </si>
   <si>
+    <t>MarineSediment</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
     <t>Coral</t>
   </si>
   <si>
-    <t>LakeSediment</t>
-  </si>
-  <si>
-    <t>MarineSediment</t>
-  </si>
-  <si>
-    <t>Documents</t>
-  </si>
-  <si>
-    <t>Speleothem</t>
-  </si>
-  <si>
     <t>MolluskShell</t>
   </si>
   <si>
     <t>Sclerosponge</t>
   </si>
   <si>
-    <t>Hybrid</t>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>Ice-other</t>
   </si>
   <si>
     <t>Midden</t>
   </si>
   <si>
-    <t>Peat</t>
-  </si>
-  <si>
-    <t>Ice-other</t>
+    <t>GroundIce</t>
   </si>
   <si>
     <t>TerrestrialSediment</t>
   </si>
   <si>
-    <t>GroundIce</t>
-  </si>
-  <si>
     <t>D18O</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>TEX86</t>
+  </si>
+  <si>
+    <t>Dd</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Blue Intensity</t>
+  </si>
+  <si>
+    <t>Tree Ring Standardized Growth Index</t>
+  </si>
+  <si>
+    <t>Layer Thickness</t>
+  </si>
+  <si>
+    <t>Maximum Latewood Density</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Biogenic Silica</t>
+  </si>
+  <si>
+    <t>Uk37</t>
+  </si>
+  <si>
+    <t>Tree Ring Width</t>
+  </si>
+  <si>
+    <t>X_Radiograph_Dark_Layer</t>
+  </si>
+  <si>
+    <t>Mass Flux</t>
+  </si>
+  <si>
+    <t>Melt</t>
+  </si>
+  <si>
+    <t>Dust</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>Trough Area Between 650 And 700 Nm Wavelength</t>
+  </si>
+  <si>
+    <t>Water Content</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C/N</t>
+  </si>
+  <si>
+    <t>Julian Day</t>
+  </si>
+  <si>
     <t>Sample Count</t>
   </si>
   <si>
     <t>Segment</t>
   </si>
   <si>
-    <t>Tree Ring Width</t>
-  </si>
-  <si>
-    <t>Tree Ring Standardized Growth Index</t>
-  </si>
-  <si>
     <t>Residual</t>
   </si>
   <si>
@@ -97,19 +175,16 @@
     <t>Rbar (Mean Pair Correlation)</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Expressed Population Signal</t>
   </si>
   <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
-  <si>
-    <t>Blue Intensity</t>
+    <t>Effective Moisture</t>
+  </si>
+  <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
+    <t>Unnamed</t>
   </si>
   <si>
     <t>D13C</t>
@@ -118,69 +193,24 @@
     <t>Sr/Ca</t>
   </si>
   <si>
-    <t>Melt</t>
-  </si>
-  <si>
-    <t>Uk37</t>
+    <t>Calcification</t>
+  </si>
+  <si>
+    <t>Composite</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Maximum Latewood Density</t>
-  </si>
-  <si>
-    <t>Julian Day</t>
-  </si>
-  <si>
     <t>Mg/Ca</t>
   </si>
   <si>
-    <t>Dd</t>
-  </si>
-  <si>
-    <t>Calcification</t>
-  </si>
-  <si>
-    <t>Composite</t>
-  </si>
-  <si>
-    <t>Precipitation</t>
-  </si>
-  <si>
-    <t>Biogenic Silica</t>
-  </si>
-  <si>
-    <t>Thickness</t>
-  </si>
-  <si>
-    <t>Unnamed</t>
-  </si>
-  <si>
-    <t>Dust</t>
-  </si>
-  <si>
-    <t>Chloride</t>
-  </si>
-  <si>
-    <t>Sulfate</t>
-  </si>
-  <si>
-    <t>Nitrate</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
     <t>Cl</t>
   </si>
   <si>
-    <t>Na</t>
-  </si>
-  <si>
     <t>Ammonium</t>
   </si>
   <si>
@@ -193,34 +223,22 @@
     <t>Ca</t>
   </si>
   <si>
-    <t>Trough Area Between 650 And 700 Nm Wavelength</t>
-  </si>
-  <si>
-    <t>Water Content</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>C/N</t>
-  </si>
-  <si>
-    <t>TEX86</t>
-  </si>
-  <si>
-    <t>X_Radiograph_Dark_Layer</t>
-  </si>
-  <si>
-    <t>Effective Moisture</t>
-  </si>
-  <si>
-    <t>Layer Thickness</t>
-  </si>
-  <si>
-    <t>Mass Flux</t>
+    <t>37:2Alkenoneconcentration</t>
+  </si>
+  <si>
+    <t>Ice Melt</t>
+  </si>
+  <si>
+    <t>Nonreliabled18O</t>
+  </si>
+  <si>
+    <t>D-Excess</t>
+  </si>
+  <si>
+    <t>Uk37'</t>
+  </si>
+  <si>
+    <t>RAN15</t>
   </si>
   <si>
     <t>Total Organic Carbon</t>
@@ -235,45 +253,27 @@
     <t>Median Grain Size (D50)</t>
   </si>
   <si>
+    <t>Mode Grain Size</t>
+  </si>
+  <si>
+    <t>Dry Bulk Density</t>
+  </si>
+  <si>
+    <t>Caco3</t>
+  </si>
+  <si>
+    <t>Meltlayers</t>
+  </si>
+  <si>
+    <t>Meltlayerfrequency</t>
+  </si>
+  <si>
     <t>BIT</t>
   </si>
   <si>
-    <t>Meltlayers</t>
-  </si>
-  <si>
-    <t>Meltlayerfrequency</t>
-  </si>
-  <si>
-    <t>Dry Bulk Density</t>
-  </si>
-  <si>
-    <t>Caco3</t>
-  </si>
-  <si>
-    <t>37:2Alkenoneconcentration</t>
-  </si>
-  <si>
-    <t>Ice Melt</t>
-  </si>
-  <si>
     <t>Bubblenumberdensity</t>
   </si>
   <si>
-    <t>Uk37'</t>
-  </si>
-  <si>
-    <t>RAN15</t>
-  </si>
-  <si>
-    <t>Nonreliabled18O</t>
-  </si>
-  <si>
-    <t>Mode Grain Size</t>
-  </si>
-  <si>
-    <t>D-Excess</t>
-  </si>
-  <si>
     <t>Brgdgt</t>
   </si>
   <si>
@@ -286,88 +286,91 @@
     <t>CBT</t>
   </si>
   <si>
+    <t>N-Alkane 24 Carbon Chain</t>
+  </si>
+  <si>
+    <t>N-Alkane 26 Carbon Chain</t>
+  </si>
+  <si>
+    <t>N-Alkane 28 Carbon Chain</t>
+  </si>
+  <si>
+    <t>Laminathickenss</t>
+  </si>
+  <si>
+    <t>Ice-Rafted Debris</t>
+  </si>
+  <si>
     <t>Foraminifera Abundance</t>
   </si>
   <si>
-    <t>Ice-Rafted Debris</t>
-  </si>
-  <si>
-    <t>Laminathickenss</t>
-  </si>
-  <si>
-    <t>N-Alkane 24 Carbon Chain</t>
-  </si>
-  <si>
-    <t>N-Alkane 26 Carbon Chain</t>
-  </si>
-  <si>
-    <t>N-Alkane 28 Carbon Chain</t>
-  </si>
-  <si>
     <t>permil</t>
   </si>
   <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>mwe</t>
+  </si>
+  <si>
+    <t>ng/g</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>mg/g</t>
+  </si>
+  <si>
+    <t>dark/sum</t>
+  </si>
+  <si>
+    <t>g/cm2a</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
     <t>count</t>
   </si>
   <si>
-    <t>cm</t>
+    <t>ppb</t>
+  </si>
+  <si>
+    <t>count/mL</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>g/cm3</t>
   </si>
   <si>
     <t>mmol/mol</t>
   </si>
   <si>
-    <t>percent</t>
-  </si>
-  <si>
-    <t>days</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>g/cm/yr</t>
   </si>
   <si>
-    <t>g/cm3</t>
+    <t>cm/yr</t>
+  </si>
+  <si>
+    <t>mm/yr</t>
   </si>
   <si>
     <t>mg/cm2/yr</t>
   </si>
   <si>
-    <t>count/mL</t>
-  </si>
-  <si>
-    <t>ppb</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>mg/g</t>
-  </si>
-  <si>
-    <t>mwe</t>
-  </si>
-  <si>
-    <t>mm/yr</t>
-  </si>
-  <si>
-    <t>degC</t>
-  </si>
-  <si>
-    <t>cm/yr</t>
-  </si>
-  <si>
-    <t>dark/sum</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>g/cm2a</t>
-  </si>
-  <si>
-    <t>ng/g</t>
+    <t>g</t>
   </si>
   <si>
     <t>unitless</t>
@@ -376,46 +379,73 @@
     <t>microm</t>
   </si>
   <si>
+    <t>microg/g</t>
+  </si>
+  <si>
     <t>decimal degrees</t>
   </si>
   <si>
+    <t>BP</t>
+  </si>
+  <si>
     <t>frequency/1000yrs</t>
   </si>
   <si>
-    <t>microg/g</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
     <t>bubbles/cm3</t>
   </si>
   <si>
-    <t>BP</t>
-  </si>
-  <si>
     <t>peak area</t>
   </si>
   <si>
     <t>permil PDB</t>
   </si>
   <si>
+    <t>no/g</t>
+  </si>
+  <si>
     <t>counts</t>
   </si>
   <si>
-    <t>no/g</t>
-  </si>
-  <si>
     <t>Precipitation Isotope</t>
   </si>
   <si>
+    <t>Water Temperature</t>
+  </si>
+  <si>
+    <t>D18O Seawater</t>
+  </si>
+  <si>
+    <t>Temperature And Precipitation</t>
+  </si>
+  <si>
+    <t>Precipitation And Evaporation</t>
+  </si>
+  <si>
+    <t>D18O Of Precipitation</t>
+  </si>
+  <si>
+    <t>Pacific Decadal Oscillation</t>
+  </si>
+  <si>
+    <t>Source Region</t>
+  </si>
+  <si>
     <t>Precipitation Amount</t>
   </si>
   <si>
-    <t>Precipitation And Evaporation</t>
-  </si>
-  <si>
-    <t>Water Temperature</t>
+    <t>Air Temperature</t>
+  </si>
+  <si>
+    <t>Lake Temperature</t>
+  </si>
+  <si>
+    <t>Relative Humidity</t>
+  </si>
+  <si>
+    <t>Evapotranspiration</t>
+  </si>
+  <si>
+    <t>Sea Ice</t>
   </si>
   <si>
     <t>Temperature And D18O Of Seawater</t>
@@ -427,124 +457,163 @@
     <t>Carbonate Ion Concentration</t>
   </si>
   <si>
-    <t>D18O Seawater</t>
+    <t>Temperature And Salinity</t>
+  </si>
+  <si>
+    <t>Atlantic Multi-Decadal Oscillation</t>
+  </si>
+  <si>
+    <t>Precipitation Seasonality</t>
+  </si>
+  <si>
+    <t>Salinity</t>
   </si>
   <si>
     <t>Palmer Drought Severity Index</t>
   </si>
   <si>
-    <t>Air Temperature</t>
-  </si>
-  <si>
-    <t>Temperature And Precipitation</t>
-  </si>
-  <si>
-    <t>D18O Of Precipitation</t>
-  </si>
-  <si>
-    <t>Source Region</t>
-  </si>
-  <si>
-    <t>Evapotranspiration</t>
-  </si>
-  <si>
-    <t>Relative Humidity</t>
-  </si>
-  <si>
-    <t>Atlantic Multi-Decadal Oscillation</t>
-  </si>
-  <si>
-    <t>Pacific Decadal Oscillation</t>
-  </si>
-  <si>
-    <t>Temperature And Salinity</t>
-  </si>
-  <si>
-    <t>Precipitation Seasonality</t>
-  </si>
-  <si>
-    <t>Salinity</t>
-  </si>
-  <si>
-    <t>Sea Ice</t>
-  </si>
-  <si>
-    <t>Lake Temperature</t>
-  </si>
-  <si>
     <t>Air Condensationlevel</t>
   </si>
   <si>
+    <t>Lake Surface</t>
+  </si>
+  <si>
     <t>Air Surface</t>
   </si>
   <si>
+    <t>Air 600M</t>
+  </si>
+  <si>
     <t>Sea Surface</t>
   </si>
   <si>
     <t>Surface</t>
   </si>
   <si>
-    <t>Lake Surface</t>
-  </si>
-  <si>
     <t>Eff</t>
   </si>
   <si>
-    <t>Air 600M</t>
-  </si>
-  <si>
     <t>Air Condensation</t>
   </si>
   <si>
     <t>Lake Water</t>
   </si>
   <si>
+    <t>Groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsurface  30M </t>
+  </si>
+  <si>
+    <t>Thermocline</t>
+  </si>
+  <si>
+    <t>Surface Mixed Layer</t>
+  </si>
+  <si>
+    <t>Near Sea Surface</t>
+  </si>
+  <si>
+    <t>Near Surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsurface  50M </t>
+  </si>
+  <si>
+    <t>Subsurface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsurface  60 80M </t>
+  </si>
+  <si>
     <t xml:space="preserve">Subsurface   50 M </t>
   </si>
   <si>
-    <t xml:space="preserve">Subsurface  30M </t>
-  </si>
-  <si>
     <t xml:space="preserve">Subsurface  300 400M </t>
   </si>
   <si>
-    <t>Subsurface</t>
-  </si>
-  <si>
-    <t>Near Surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subsurface  50M </t>
-  </si>
-  <si>
-    <t>Thermocline</t>
-  </si>
-  <si>
-    <t>Near Sea Surface</t>
-  </si>
-  <si>
-    <t>Groundwater</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subsurface  60 80M </t>
-  </si>
-  <si>
-    <t>Surface Mixed Layer</t>
+    <t>Subsurface  136 M</t>
   </si>
   <si>
     <t>Subsurface  143 M</t>
   </si>
   <si>
-    <t>Subsurface  136 M</t>
+    <t>Sea Surface  Temperature</t>
+  </si>
+  <si>
+    <t>Sea Surface D18O Seawater</t>
+  </si>
+  <si>
+    <t>Sea Surface Temperature And Precipitation</t>
   </si>
   <si>
     <t>Lake Water Temperature</t>
   </si>
   <si>
-    <t>Sea Surface  Temperature</t>
-  </si>
-  <si>
-    <t>Sea Surface D18O Seawater</t>
+    <t>Precipitation D18O</t>
+  </si>
+  <si>
+    <t>Thermocline Temperature And D18O Of Seawater</t>
+  </si>
+  <si>
+    <t>Thermocline  Temperature</t>
+  </si>
+  <si>
+    <t>Thermocline Seawater Isotope</t>
+  </si>
+  <si>
+    <t>Thermocline Carbonate Ion Concentration</t>
+  </si>
+  <si>
+    <t>Surface Mixed Layer Temperature And D18O Of Seawater</t>
+  </si>
+  <si>
+    <t>Surface Mixed Layer  Temperature</t>
+  </si>
+  <si>
+    <t>Surface Mixed Layer Seawater Isotope</t>
+  </si>
+  <si>
+    <t>Surface Mixed Layer Carbonate Ion Concentration</t>
+  </si>
+  <si>
+    <t>Near Sea Surface Temperature And D18O Of Seawater</t>
+  </si>
+  <si>
+    <t>Near Sea Surface  Temperature</t>
+  </si>
+  <si>
+    <t>Near Sea Surface Seawater Isotope</t>
+  </si>
+  <si>
+    <t>Near Sea Surface Carbonate Ion Concentration</t>
+  </si>
+  <si>
+    <t>Surface Temperature And D18O Of Seawater</t>
+  </si>
+  <si>
+    <t>Surface Seawater Isotope</t>
+  </si>
+  <si>
+    <t>Sea Surface Carbonate Ion Concentration</t>
+  </si>
+  <si>
+    <t>Near Surface Temperature And D18O Of Seawater</t>
+  </si>
+  <si>
+    <t>Near Surface  Temperature</t>
+  </si>
+  <si>
+    <t>Near Surface Seawater Isotope</t>
+  </si>
+  <si>
+    <t>Near Surface Carbonate Ion Concentration</t>
+  </si>
+  <si>
+    <t>Sea Surface Temperature And D18O Of Seawater</t>
+  </si>
+  <si>
+    <t>Sea Surface Seawater Isotope</t>
   </si>
   <si>
     <t>Subsurface  Temperature</t>
@@ -556,94 +625,22 @@
     <t>Subsurface Carbonate Ion Concentration</t>
   </si>
   <si>
-    <t>Sea Surface Temperature And D18O Of Seawater</t>
-  </si>
-  <si>
-    <t>Sea Surface Seawater Isotope</t>
-  </si>
-  <si>
-    <t>Sea Surface Carbonate Ion Concentration</t>
-  </si>
-  <si>
-    <t>Surface Temperature And D18O Of Seawater</t>
-  </si>
-  <si>
-    <t>Surface Seawater Isotope</t>
-  </si>
-  <si>
-    <t>Near Surface Temperature And D18O Of Seawater</t>
-  </si>
-  <si>
-    <t>Near Surface  Temperature</t>
-  </si>
-  <si>
-    <t>Near Surface Seawater Isotope</t>
-  </si>
-  <si>
-    <t>Near Surface Carbonate Ion Concentration</t>
-  </si>
-  <si>
-    <t>Thermocline Temperature And D18O Of Seawater</t>
-  </si>
-  <si>
-    <t>Thermocline  Temperature</t>
-  </si>
-  <si>
-    <t>Thermocline Seawater Isotope</t>
-  </si>
-  <si>
-    <t>Thermocline Carbonate Ion Concentration</t>
-  </si>
-  <si>
-    <t>Near Sea Surface Temperature And D18O Of Seawater</t>
-  </si>
-  <si>
-    <t>Near Sea Surface  Temperature</t>
-  </si>
-  <si>
-    <t>Near Sea Surface Seawater Isotope</t>
-  </si>
-  <si>
-    <t>Near Sea Surface Carbonate Ion Concentration</t>
-  </si>
-  <si>
-    <t>Precipitation D18O</t>
-  </si>
-  <si>
-    <t>Sea Surface Temperature And Precipitation</t>
-  </si>
-  <si>
     <t>Sea Surface Temperature And Salinity</t>
   </si>
   <si>
-    <t>Surface Mixed Layer Temperature And D18O Of Seawater</t>
-  </si>
-  <si>
-    <t>Surface Mixed Layer  Temperature</t>
-  </si>
-  <si>
-    <t>Surface Mixed Layer Seawater Isotope</t>
-  </si>
-  <si>
-    <t>Surface Mixed Layer Carbonate Ion Concentration</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
+    <t>Sedimentation Rate</t>
+  </si>
+  <si>
+    <t>Sea Surface Temperature</t>
+  </si>
+  <si>
     <t>Subsurface Temperature</t>
   </si>
   <si>
-    <t>Sedimentation Rate</t>
-  </si>
-  <si>
-    <t>Sea Surface Temperature</t>
-  </si>
-  <si>
     <t>cm/kyr</t>
-  </si>
-  <si>
-    <t>PC</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>492</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1034,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1944</v>
+        <v>553</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1045,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>314</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1056,7 +1053,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>553</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1089,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>160</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1100,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1111,7 +1108,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1122,7 +1119,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1133,7 +1130,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>54</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1144,7 +1141,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>125</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1155,7 +1152,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>16</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1166,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1177,7 +1174,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1217,7 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>127</v>
+        <v>624</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1231,7 +1228,7 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1242,7 +1239,7 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>124</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1253,7 +1250,7 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>375</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1264,7 +1261,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>126</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1275,7 +1272,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>126</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1286,7 +1283,7 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <v>126</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1297,7 +1294,7 @@
         <v>24</v>
       </c>
       <c r="C10">
-        <v>126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1308,7 +1305,7 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>741</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1319,7 +1316,7 @@
         <v>26</v>
       </c>
       <c r="C12">
-        <v>126</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1330,7 +1327,7 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>132</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1341,7 +1338,7 @@
         <v>28</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1352,7 +1349,7 @@
         <v>29</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1363,7 +1360,7 @@
         <v>30</v>
       </c>
       <c r="C16">
-        <v>355</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1374,7 +1371,7 @@
         <v>31</v>
       </c>
       <c r="C17">
-        <v>24</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1385,7 +1382,7 @@
         <v>32</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1396,7 +1393,7 @@
         <v>33</v>
       </c>
       <c r="C19">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1407,7 +1404,7 @@
         <v>34</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1418,7 +1415,7 @@
         <v>35</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1440,7 +1437,7 @@
         <v>37</v>
       </c>
       <c r="C23">
-        <v>111</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1451,7 +1448,7 @@
         <v>38</v>
       </c>
       <c r="C24">
-        <v>227</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1462,7 +1459,7 @@
         <v>39</v>
       </c>
       <c r="C25">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1473,7 +1470,7 @@
         <v>40</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1484,7 +1481,7 @@
         <v>41</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1495,7 +1492,7 @@
         <v>42</v>
       </c>
       <c r="C28">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1506,7 +1503,7 @@
         <v>43</v>
       </c>
       <c r="C29">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1517,7 +1514,7 @@
         <v>44</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1528,7 +1525,7 @@
         <v>45</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1539,7 +1536,7 @@
         <v>46</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1550,7 +1547,7 @@
         <v>47</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1561,7 +1558,7 @@
         <v>48</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1572,7 +1569,7 @@
         <v>49</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1583,7 +1580,7 @@
         <v>50</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1594,7 +1591,7 @@
         <v>51</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1627,7 +1624,7 @@
         <v>54</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1638,7 +1635,7 @@
         <v>55</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1649,7 +1646,7 @@
         <v>56</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1660,7 +1657,7 @@
         <v>57</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1671,7 +1668,7 @@
         <v>58</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1682,7 +1679,7 @@
         <v>59</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1693,7 +1690,7 @@
         <v>60</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1715,7 +1712,7 @@
         <v>62</v>
       </c>
       <c r="C48">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1726,7 +1723,7 @@
         <v>63</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1737,7 +1734,7 @@
         <v>64</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1748,7 +1745,7 @@
         <v>65</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1759,7 +1756,7 @@
         <v>66</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1770,7 +1767,7 @@
         <v>67</v>
       </c>
       <c r="C53">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1803,7 +1800,7 @@
         <v>70</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1814,7 +1811,7 @@
         <v>71</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1825,7 +1822,7 @@
         <v>72</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1836,7 +1833,7 @@
         <v>73</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1847,7 +1844,7 @@
         <v>74</v>
       </c>
       <c r="C60">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1858,7 +1855,7 @@
         <v>75</v>
       </c>
       <c r="C61">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1869,7 +1866,7 @@
         <v>76</v>
       </c>
       <c r="C62">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1880,7 +1877,7 @@
         <v>77</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1891,7 +1888,7 @@
         <v>78</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1902,7 +1899,7 @@
         <v>79</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1913,7 +1910,7 @@
         <v>80</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1935,7 +1932,7 @@
         <v>82</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1946,7 +1943,7 @@
         <v>83</v>
       </c>
       <c r="C69">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2001,7 +1998,7 @@
         <v>88</v>
       </c>
       <c r="C74">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2012,7 +2009,7 @@
         <v>89</v>
       </c>
       <c r="C75">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2023,7 +2020,7 @@
         <v>90</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2034,7 +2031,7 @@
         <v>91</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2045,7 +2042,7 @@
         <v>92</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2056,7 +2053,7 @@
         <v>93</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2099,7 +2096,7 @@
         <v>95</v>
       </c>
       <c r="C3">
-        <v>129</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2107,10 +2104,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>1780</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2132,7 +2129,7 @@
         <v>97</v>
       </c>
       <c r="C6">
-        <v>108</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2143,7 +2140,7 @@
         <v>98</v>
       </c>
       <c r="C7">
-        <v>146</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2154,7 +2151,7 @@
         <v>99</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2176,7 +2173,7 @@
         <v>101</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2187,7 +2184,7 @@
         <v>102</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2198,7 +2195,7 @@
         <v>103</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2220,7 +2217,7 @@
         <v>105</v>
       </c>
       <c r="C14">
-        <v>24</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2231,7 +2228,7 @@
         <v>106</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2242,7 +2239,7 @@
         <v>107</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2253,7 +2250,7 @@
         <v>108</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2264,7 +2261,7 @@
         <v>109</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2275,7 +2272,7 @@
         <v>110</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2286,7 +2283,7 @@
         <v>111</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2297,7 +2294,7 @@
         <v>112</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2308,7 +2305,7 @@
         <v>113</v>
       </c>
       <c r="C22">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2330,7 +2327,7 @@
         <v>115</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2341,7 +2338,7 @@
         <v>116</v>
       </c>
       <c r="C25">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2352,7 +2349,7 @@
         <v>117</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2363,7 +2360,7 @@
         <v>118</v>
       </c>
       <c r="C27">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2374,7 +2371,7 @@
         <v>119</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2385,7 +2382,7 @@
         <v>120</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2396,7 +2393,7 @@
         <v>121</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2407,7 +2404,7 @@
         <v>122</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2418,7 +2415,7 @@
         <v>123</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2451,7 +2448,7 @@
         <v>126</v>
       </c>
       <c r="C35">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2462,7 +2459,7 @@
         <v>127</v>
       </c>
       <c r="C36">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2491,10 +2488,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>4328</v>
+        <v>4211</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2516,7 +2513,7 @@
         <v>129</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2527,7 +2524,7 @@
         <v>130</v>
       </c>
       <c r="C5">
-        <v>117</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2538,7 +2535,7 @@
         <v>131</v>
       </c>
       <c r="C6">
-        <v>171</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2549,7 +2546,7 @@
         <v>132</v>
       </c>
       <c r="C7">
-        <v>69</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2560,7 +2557,7 @@
         <v>133</v>
       </c>
       <c r="C8">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2571,7 +2568,7 @@
         <v>134</v>
       </c>
       <c r="C9">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2582,7 +2579,7 @@
         <v>135</v>
       </c>
       <c r="C10">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2593,7 +2590,7 @@
         <v>136</v>
       </c>
       <c r="C11">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2615,7 +2612,7 @@
         <v>138</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2626,7 +2623,7 @@
         <v>139</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2637,7 +2634,7 @@
         <v>140</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2648,7 +2645,7 @@
         <v>141</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2659,7 +2656,7 @@
         <v>142</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2670,7 +2667,7 @@
         <v>143</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2681,7 +2678,7 @@
         <v>144</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2714,7 +2711,7 @@
         <v>147</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2725,7 +2722,7 @@
         <v>148</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2736,7 +2733,7 @@
         <v>149</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2776,10 +2773,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>3910</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2790,7 +2787,7 @@
         <v>151</v>
       </c>
       <c r="C4">
-        <v>802</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2801,7 +2798,7 @@
         <v>152</v>
       </c>
       <c r="C5">
-        <v>316</v>
+        <v>802</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2812,7 +2809,7 @@
         <v>153</v>
       </c>
       <c r="C6">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2823,7 +2820,7 @@
         <v>154</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2834,7 +2831,7 @@
         <v>155</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2845,7 +2842,7 @@
         <v>156</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2878,7 +2875,7 @@
         <v>159</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2900,7 +2897,7 @@
         <v>161</v>
       </c>
       <c r="C14">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2911,7 +2908,7 @@
         <v>162</v>
       </c>
       <c r="C15">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2922,7 +2919,7 @@
         <v>163</v>
       </c>
       <c r="C16">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2933,7 +2930,7 @@
         <v>164</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2944,7 +2941,7 @@
         <v>165</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2955,7 +2952,7 @@
         <v>166</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2966,7 +2963,7 @@
         <v>167</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2988,7 +2985,7 @@
         <v>169</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3039,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>4304</v>
@@ -3061,10 +3058,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C4">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3072,10 +3069,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3083,10 +3080,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>174</v>
       </c>
       <c r="C6">
-        <v>151</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3094,10 +3091,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3105,10 +3102,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C8">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3116,10 +3113,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3127,10 +3124,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3138,10 +3135,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3149,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3160,10 +3157,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3171,10 +3168,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C14">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3182,10 +3179,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -3193,10 +3190,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3204,10 +3201,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3215,10 +3212,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3226,10 +3223,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3237,10 +3234,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3248,10 +3245,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>185</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3259,7 +3256,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3270,7 +3267,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -3281,7 +3278,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -3292,10 +3289,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3303,10 +3300,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3314,10 +3311,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3325,10 +3322,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3336,10 +3333,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -3347,10 +3344,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -3358,10 +3355,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>195</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3372,7 +3369,7 @@
         <v>196</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3380,10 +3377,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3391,10 +3388,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3402,10 +3399,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3413,10 +3410,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3424,7 +3421,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3435,7 +3432,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>139</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3449,7 +3446,7 @@
         <v>202</v>
       </c>
       <c r="C39">
-        <v>383</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3492,7 +3489,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3511,10 +3508,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>4776</v>
+        <v>4774</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3522,10 +3519,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C3">
-        <v>383</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3547,40 +3544,7 @@
         <v>94</v>
       </c>
       <c r="C5">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>